<commit_message>
2.10.8 back to original gyro corr+less input
</commit_message>
<xml_diff>
--- a/doc/IMU_orientation.xlsx
+++ b/doc/IMU_orientation.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20055" windowHeight="9480"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="20055" windowHeight="9480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId2"/>
+    <sheet name="roll rate" sheetId="4" r:id="rId3"/>
+    <sheet name="ptich rate" sheetId="5" r:id="rId4"/>
+    <sheet name="roll stabilize" sheetId="6" r:id="rId5"/>
+    <sheet name="pitch stabilize" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="157">
   <si>
     <t>y+</t>
   </si>
@@ -258,13 +262,241 @@
   </si>
   <si>
     <t xml:space="preserve">plane has nose up (row 3) </t>
+  </si>
+  <si>
+    <t>Gyrox</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>when plane</t>
+  </si>
+  <si>
+    <t>left wing</t>
+  </si>
+  <si>
+    <t>right wing</t>
+  </si>
+  <si>
+    <t>&gt;0</t>
+  </si>
+  <si>
+    <t>&lt;0</t>
+  </si>
+  <si>
+    <t>sign of mpu</t>
+  </si>
+  <si>
+    <t>sign of convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for openTx</t>
+  </si>
+  <si>
+    <t>depends on servo and mecanical setup</t>
+  </si>
+  <si>
+    <t>during mixer calib with stick right</t>
+  </si>
+  <si>
+    <t>centered</t>
+  </si>
+  <si>
+    <t>ail stick (pwm us)</t>
+  </si>
+  <si>
+    <t>servo ail (pwm us)</t>
+  </si>
+  <si>
+    <t>dirch[] (=stick position right corner)</t>
+  </si>
+  <si>
+    <t>rightup servo position</t>
+  </si>
+  <si>
+    <t>leftdown servo position</t>
+  </si>
+  <si>
+    <t>rateRollRightUs</t>
+  </si>
+  <si>
+    <t>rateRollLeftUs</t>
+  </si>
+  <si>
+    <t>In rate mode with stick centerd, imagine left wing goes up, so plane goes to right and gyroX is &gt;0</t>
+  </si>
+  <si>
+    <t>gyrox</t>
+  </si>
+  <si>
+    <t>(max is 32768)</t>
+  </si>
+  <si>
+    <t>stickAilUs_offset</t>
+  </si>
+  <si>
+    <t>stickAilUs (= position of stick)</t>
+  </si>
+  <si>
+    <t>stick gain max</t>
+  </si>
+  <si>
+    <t>shift = stick gain throw-1</t>
+  </si>
+  <si>
+    <t>abs(stickoffset)&lt;&lt;shift</t>
+  </si>
+  <si>
+    <t>min (abs,max)</t>
+  </si>
+  <si>
+    <t>stick gain = max -min()</t>
+  </si>
+  <si>
+    <t>Master gain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> between 0 and 512</t>
+  </si>
+  <si>
+    <t>input = -gyroX</t>
+  </si>
+  <si>
+    <t>setpoint</t>
+  </si>
+  <si>
+    <t>PID in rate mode</t>
+  </si>
+  <si>
+    <t>err = input-setpoint</t>
+  </si>
+  <si>
+    <t>last err</t>
+  </si>
+  <si>
+    <t>diff err = err - last err</t>
+  </si>
+  <si>
+    <t>kp</t>
+  </si>
+  <si>
+    <t>kd</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>correction</t>
+  </si>
+  <si>
+    <t>Vr gain</t>
+  </si>
+  <si>
+    <t>nose</t>
+  </si>
+  <si>
+    <t>when nose</t>
+  </si>
+  <si>
+    <t>queue</t>
+  </si>
+  <si>
+    <t>Gyroy</t>
+  </si>
+  <si>
+    <t>pitch</t>
+  </si>
+  <si>
+    <t>pitch  stick (pwm us)</t>
+  </si>
+  <si>
+    <t>dirch[] (=stick position up corner)</t>
+  </si>
+  <si>
+    <t>gyroy</t>
+  </si>
+  <si>
+    <t>In rate mode with stick centerd, imagine left noes  goes up, so gyroY is &lt;0</t>
+  </si>
+  <si>
+    <t>ratePitchUpUs</t>
+  </si>
+  <si>
+    <t>ratePitchDownUs</t>
+  </si>
+  <si>
+    <t>OSP (original stick pos</t>
+  </si>
+  <si>
+    <t>ESP (expected stick position)</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>cn</t>
+  </si>
+  <si>
+    <t>servo poswithout cor</t>
+  </si>
+  <si>
+    <t>with correction</t>
+  </si>
+  <si>
+    <t>input = gyroY</t>
+  </si>
+  <si>
+    <t>output (err*kp/8 + diffErr*kd/4)/256</t>
+  </si>
+  <si>
+    <t>correction (out*Vr*stick*mast gains)</t>
+  </si>
+  <si>
+    <t>correction positive</t>
+  </si>
+  <si>
+    <t>correction negative</t>
+  </si>
+  <si>
+    <t>In stab mode with stick centered, imagine left wing is up, so plane goes to right and Roll is &gt;0</t>
+  </si>
+  <si>
+    <t>Roll in 1/10 of deg</t>
+  </si>
+  <si>
+    <t>during mixer calib with stick nose up</t>
+  </si>
+  <si>
+    <t>pitch in 1/10 of deg</t>
+  </si>
+  <si>
+    <t>pitch scaled (&lt;&lt; 1)</t>
+  </si>
+  <si>
+    <t>input = pitch scaled</t>
+  </si>
+  <si>
+    <t>input = Roll scaled</t>
+  </si>
+  <si>
+    <t>Roll scaled (&lt;&lt; 1)</t>
+  </si>
+  <si>
+    <t>In stab mode with stick centered, imagine nose is  DOWN and pitch is &lt;0</t>
+  </si>
+  <si>
+    <t>Inverted !!!!!!!!</t>
+  </si>
+  <si>
+    <t>NOT inverted !!!!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,13 +504,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -293,8 +545,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E13:E47" si="2">CONCATENATE(G14,"_",H14)</f>
+        <f t="shared" ref="E14:E45" si="2">CONCATENATE(G14,"_",H14)</f>
         <v>front_left</v>
       </c>
       <c r="G14" t="s">
@@ -3011,4 +3267,1816 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C8">
+        <v>1500</v>
+      </c>
+      <c r="D8">
+        <v>988</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1900</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
+        <v>1200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <f>B8</f>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <f>B10</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <f>D10</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <f>B14-C10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <f>B15-C10</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1">
+        <v>32700</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <f>B23-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27">
+        <f>ABS(B24)*POWER(2,B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28">
+        <f>MIN(B27,B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
+        <f>B25-B28</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31">
+        <v>400</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34">
+        <v>500</v>
+      </c>
+      <c r="F34" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>B35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36">
+        <f>-B21</f>
+        <v>-32700</v>
+      </c>
+      <c r="C36">
+        <f>B36</f>
+        <v>-32700</v>
+      </c>
+      <c r="E36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>B38</f>
+        <v>-32700</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <f>B36-B35</f>
+        <v>-32700</v>
+      </c>
+      <c r="C38">
+        <f>C36-C35</f>
+        <v>-32700</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>-32700</v>
+      </c>
+      <c r="C39">
+        <f>C38-C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40">
+        <f>INT( (B38*$E$34/8+B39*$G$34/4)/POWER(2,8))</f>
+        <v>-23951</v>
+      </c>
+      <c r="C40">
+        <f>INT( (C38*$E$34/8+C39*$G$34/4)/POWER(2,8))</f>
+        <v>-7984</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41">
+        <f>INT(B40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>-14505</v>
+      </c>
+      <c r="C41">
+        <f>INT(C40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>-4835</v>
+      </c>
+      <c r="E41" t="str">
+        <f>IF((B41*B16) &gt; 0, "OK", "wrong")</f>
+        <v>wrong</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43">
+        <f>$B$23</f>
+        <v>1500</v>
+      </c>
+      <c r="C43">
+        <f>$B$23</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44">
+        <f>B43+B41</f>
+        <v>-13005</v>
+      </c>
+      <c r="C44">
+        <f>C43+C41</f>
+        <v>-3335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45">
+        <f>IF(B43&gt;=1500,IF(B44&gt;=1500,B41,1500-B43),IF(B44&gt;=1500,B44-1500,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f>IF(C43&gt;=1500,IF(C44&gt;=1500,C41,1500-C43),IF(C44&gt;=1500,C44-1500,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46">
+        <f>B41-B45</f>
+        <v>-14505</v>
+      </c>
+      <c r="C46">
+        <f>C41-C45</f>
+        <v>-4835</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48">
+        <v>1500</v>
+      </c>
+      <c r="C48">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49">
+        <f>INT(B48+(B45*$B$16)/POWER(2,9) - B46*$B$17/POWER(2,9))</f>
+        <v>-7000</v>
+      </c>
+      <c r="C49">
+        <f>INT(C48+(C45*$B$16)/POWER(2,9) - C46*$B$17/POWER(2,9))</f>
+        <v>-1334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="1">
+        <v>988</v>
+      </c>
+      <c r="C8">
+        <v>1500</v>
+      </c>
+      <c r="D8">
+        <v>2012</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
+        <v>1900</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <f>B8</f>
+        <v>988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <f>B10</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <f>D10</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16">
+        <f>B14-C10</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17">
+        <f>B15-C10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <f>B23-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27">
+        <f>ABS(B24)*POWER(2,B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28">
+        <f>MIN(B27,B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
+        <f>B25-B28</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="1">
+        <v>400</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34">
+        <v>500</v>
+      </c>
+      <c r="F34" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>B35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36">
+        <f>B21</f>
+        <v>-1000</v>
+      </c>
+      <c r="C36">
+        <f>B36</f>
+        <v>-1000</v>
+      </c>
+      <c r="E36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>B38</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <f>B36-B35</f>
+        <v>-1000</v>
+      </c>
+      <c r="C38">
+        <f>C36-C35</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>-1000</v>
+      </c>
+      <c r="C39">
+        <f>C38-C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40">
+        <f>INT( (B38*$E$34/8+B39*$G$34/4)/POWER(2,8))</f>
+        <v>-733</v>
+      </c>
+      <c r="C40">
+        <f>INT( (C38*$E$34/8+C39*$G$34/4)/POWER(2,8))</f>
+        <v>-245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41">
+        <f>INT(B40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>-444</v>
+      </c>
+      <c r="C41">
+        <f>INT(C40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>-149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43">
+        <f>$B$23</f>
+        <v>1500</v>
+      </c>
+      <c r="C43">
+        <f>$B$23</f>
+        <v>1500</v>
+      </c>
+      <c r="D43">
+        <f>MAX(B43,$D$10)</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44">
+        <f>B43+B41</f>
+        <v>1056</v>
+      </c>
+      <c r="C44">
+        <f>C43+C41</f>
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45">
+        <f>IF(B43&gt;=1500,IF(B44&gt;=1500,B41,1500-B43),IF(B44&gt;=1500,B44-1500,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f>IF(C43&gt;=1500,IF(C44&gt;=1500,C41,1500-C43),IF(C44&gt;=1500,C44-1500,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46">
+        <f>B41-B45</f>
+        <v>-444</v>
+      </c>
+      <c r="C46">
+        <f>C41-C45</f>
+        <v>-149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48">
+        <v>1500</v>
+      </c>
+      <c r="C48">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49">
+        <f>INT(B48+(B45*$B$16)/POWER(2,9) - B46*$B$17/POWER(2,9))</f>
+        <v>1846</v>
+      </c>
+      <c r="C49">
+        <f>INT(C48+(C45*$B$16)/POWER(2,9) - C46*$B$17/POWER(2,9))</f>
+        <v>1616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C8">
+        <v>1500</v>
+      </c>
+      <c r="D8">
+        <v>988</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1900</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
+        <v>1200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <f>B8</f>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <f>B10</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <f>D10</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <f>B14-C10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <f>B15-C10</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B21*POWER(2,1)</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25">
+        <f>B24-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28">
+        <f>ABS(B25)*POWER(2,B27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <f>MIN(B28,B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30">
+        <f>B26-B29</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32">
+        <v>400</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35">
+        <v>500</v>
+      </c>
+      <c r="F35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>B36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37">
+        <f>-B22</f>
+        <v>-1200</v>
+      </c>
+      <c r="C37">
+        <f>B37</f>
+        <v>-1200</v>
+      </c>
+      <c r="E37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>B39</f>
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39">
+        <f>B37-B36</f>
+        <v>-1200</v>
+      </c>
+      <c r="C39">
+        <f>C37-C36</f>
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40">
+        <f>B39-B38</f>
+        <v>-1200</v>
+      </c>
+      <c r="C40">
+        <f>C39-C38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41">
+        <f>INT( (B39*$E$35/8+B40*$G$35/4)/POWER(2,8))</f>
+        <v>-879</v>
+      </c>
+      <c r="C41">
+        <f>INT( (C39*$E$35/8+C40*$G$35/4)/POWER(2,8))</f>
+        <v>-293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42">
+        <f>INT(B41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
+        <v>-533</v>
+      </c>
+      <c r="C42">
+        <f>INT(C41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
+        <v>-178</v>
+      </c>
+      <c r="E42" t="str">
+        <f>IF((B42*B21) &lt; 0, "OK", "wrong")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44">
+        <f>$B$24</f>
+        <v>1500</v>
+      </c>
+      <c r="C44">
+        <f>$B$24</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45">
+        <f>B44+B42</f>
+        <v>967</v>
+      </c>
+      <c r="C45">
+        <f>C44+C42</f>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46">
+        <f>IF(B44&gt;=1500,IF(B45&gt;=1500,B42,1500-B44),IF(B45&gt;=1500,B45-1500,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f>IF(C44&gt;=1500,IF(C45&gt;=1500,C42,1500-C44),IF(C45&gt;=1500,C45-1500,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47">
+        <f>B42-B46</f>
+        <v>-533</v>
+      </c>
+      <c r="C47">
+        <f>C42-C46</f>
+        <v>-178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49">
+        <v>1500</v>
+      </c>
+      <c r="C49">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50">
+        <f>INT(B49+(B46*$B$16)/POWER(2,9) - B47*$B$17/POWER(2,9))</f>
+        <v>1187</v>
+      </c>
+      <c r="C50">
+        <f>INT(C49+(C46*$B$16)/POWER(2,9) - C47*$B$17/POWER(2,9))</f>
+        <v>1395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="1">
+        <v>988</v>
+      </c>
+      <c r="C8">
+        <v>1500</v>
+      </c>
+      <c r="D8">
+        <v>2012</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
+        <v>1900</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <f>B8</f>
+        <v>988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <f>B10</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <f>D10</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <f>B14-C10</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <f>B15-C10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21">
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="1">
+        <f>B21*POWER(2,1)</f>
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25">
+        <f>B24-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28">
+        <f>ABS(B25)*POWER(2,B27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <f>MIN(B28,B26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30">
+        <f>B26-B29</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32">
+        <v>400</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35">
+        <v>500</v>
+      </c>
+      <c r="F35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>B36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37">
+        <f>-B22</f>
+        <v>1200</v>
+      </c>
+      <c r="C37">
+        <f>B37</f>
+        <v>1200</v>
+      </c>
+      <c r="E37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>B39</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39">
+        <f>B37-B36</f>
+        <v>1200</v>
+      </c>
+      <c r="C39">
+        <f>C37-C36</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40">
+        <f>B39-B38</f>
+        <v>1200</v>
+      </c>
+      <c r="C40">
+        <f>C39-C38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41">
+        <f>INT( (B39*$E$35/8+B40*$G$35/4)/POWER(2,8))</f>
+        <v>878</v>
+      </c>
+      <c r="C41">
+        <f>INT( (C39*$E$35/8+C40*$G$35/4)/POWER(2,8))</f>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42">
+        <f>INT(B41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
+        <v>531</v>
+      </c>
+      <c r="C42">
+        <f>INT(C41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
+        <v>176</v>
+      </c>
+      <c r="E42" s="4" t="str">
+        <f>IF((B42*B21) &lt; 0, "OK", "wrong")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44">
+        <f>$B$24</f>
+        <v>1500</v>
+      </c>
+      <c r="C44">
+        <f>$B$24</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45">
+        <f>B44+B42</f>
+        <v>2031</v>
+      </c>
+      <c r="C45">
+        <f>C44+C42</f>
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46">
+        <f>IF(B44&gt;=1500,IF(B45&gt;=1500,B42,1500-B44),IF(B45&gt;=1500,B45-1500,0))</f>
+        <v>531</v>
+      </c>
+      <c r="C46">
+        <f>IF(C44&gt;=1500,IF(C45&gt;=1500,C42,1500-C44),IF(C45&gt;=1500,C45-1500,0))</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47">
+        <f>B42-B46</f>
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <f>C42-C46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49">
+        <v>1500</v>
+      </c>
+      <c r="C49">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B50">
+        <f>INT(B49+(B46*$B$16)/POWER(2,9) - B47*$B$17/POWER(2,9))</f>
+        <v>1188</v>
+      </c>
+      <c r="C50">
+        <f>INT(C49+(C46*$B$16)/POWER(2,9) - C47*$B$17/POWER(2,9))</f>
+        <v>1396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2.10.9 checks imu calib+no corr high roll/pitch
</commit_message>
<xml_diff>
--- a/doc/IMU_orientation.xlsx
+++ b/doc/IMU_orientation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20055" windowHeight="9480" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="20055" windowHeight="9480" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="ptich rate" sheetId="5" r:id="rId4"/>
     <sheet name="roll stabilize" sheetId="6" r:id="rId5"/>
     <sheet name="pitch stabilize" sheetId="7" r:id="rId6"/>
+    <sheet name="roll hold" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="163">
   <si>
     <t>y+</t>
   </si>
@@ -490,6 +491,24 @@
   </si>
   <si>
     <t>NOT inverted !!!!!!</t>
+  </si>
+  <si>
+    <t>Note= yellow = cell can be introduced</t>
+  </si>
+  <si>
+    <t>In Hold mode with stick centerd, imagine left wing goes up, so plane goes to right and gyroX is &gt;0</t>
+  </si>
+  <si>
+    <t>!!!!!!!!!!!!!! Not yet filled for HOLD mode (KI + setpoint are differentµ</t>
+  </si>
+  <si>
+    <t>max rotate gain</t>
+  </si>
+  <si>
+    <t>setpoint = -stickAilUs_offset&lt;&lt;max rotate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &gt;0 is stick to right</t>
   </si>
 </sst>
 </file>
@@ -545,12 +564,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3273,8 +3293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3282,7 +3302,7 @@
     <col min="1" max="1" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3295,8 +3315,11 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -3307,7 +3330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3318,7 +3341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -3332,7 +3355,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -3346,46 +3369,46 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="1">
         <v>2012</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1500</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>988</v>
       </c>
       <c r="E8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="1">
         <v>1900</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>1500</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1200</v>
       </c>
       <c r="E10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -3394,7 +3417,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -3403,7 +3426,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -3412,7 +3435,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -3431,7 +3454,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3632,10 +3655,6 @@
       <c r="C41">
         <f>INT(C40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
         <v>-4835</v>
-      </c>
-      <c r="E41" t="str">
-        <f>IF((B41*B16) &gt; 0, "OK", "wrong")</f>
-        <v>wrong</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3723,7 +3742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
@@ -4173,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4253,10 +4272,10 @@
       <c r="B8" s="1">
         <v>2012</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>1500</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>988</v>
       </c>
       <c r="E8" t="s">
@@ -4268,13 +4287,13 @@
         <v>95</v>
       </c>
       <c r="B10" s="1">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="C10">
         <v>1500</v>
       </c>
-      <c r="D10">
-        <v>1200</v>
+      <c r="D10" s="1">
+        <v>1000</v>
       </c>
       <c r="E10" t="s">
         <v>91</v>
@@ -4300,7 +4319,7 @@
       </c>
       <c r="B14">
         <f>B10</f>
-        <v>1900</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4309,7 +4328,7 @@
       </c>
       <c r="B15">
         <f>D10</f>
-        <v>1200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4318,7 +4337,7 @@
       </c>
       <c r="B16">
         <f>B14-C10</f>
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4327,7 +4346,7 @@
       </c>
       <c r="B17">
         <f>B15-C10</f>
-        <v>-300</v>
+        <v>-500</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4339,17 +4358,17 @@
       <c r="A21" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B21">
-        <v>600</v>
+      <c r="B21" s="1">
+        <v>900</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <f>B21*POWER(2,1)</f>
-        <v>1200</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4466,11 +4485,11 @@
       </c>
       <c r="B37">
         <f>-B22</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
       <c r="C37">
         <f>B37</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
       <c r="E37" t="s">
         <v>155</v>
@@ -4485,7 +4504,7 @@
       </c>
       <c r="C38">
         <f>B39</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -4494,11 +4513,11 @@
       </c>
       <c r="B39">
         <f>B37-B36</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
       <c r="C39">
         <f>C37-C36</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -4507,7 +4526,7 @@
       </c>
       <c r="B40">
         <f>B39-B38</f>
-        <v>-1200</v>
+        <v>-1800</v>
       </c>
       <c r="C40">
         <f>C39-C38</f>
@@ -4520,11 +4539,11 @@
       </c>
       <c r="B41">
         <f>INT( (B39*$E$35/8+B40*$G$35/4)/POWER(2,8))</f>
-        <v>-879</v>
+        <v>-1319</v>
       </c>
       <c r="C41">
         <f>INT( (C39*$E$35/8+C40*$G$35/4)/POWER(2,8))</f>
-        <v>-293</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -4533,13 +4552,13 @@
       </c>
       <c r="B42">
         <f>INT(B41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
-        <v>-533</v>
+        <v>-799</v>
       </c>
       <c r="C42">
         <f>INT(C41*$B$33/POWER(2,7)*$B$30/POWER(2,9)*$B$32/POWER(2,9))</f>
-        <v>-178</v>
-      </c>
-      <c r="E42" t="str">
+        <v>-267</v>
+      </c>
+      <c r="E42" s="4" t="str">
         <f>IF((B42*B21) &lt; 0, "OK", "wrong")</f>
         <v>OK</v>
       </c>
@@ -4563,11 +4582,11 @@
       </c>
       <c r="B45">
         <f>B44+B42</f>
-        <v>967</v>
+        <v>701</v>
       </c>
       <c r="C45">
         <f>C44+C42</f>
-        <v>1322</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -4589,11 +4608,11 @@
       </c>
       <c r="B47">
         <f>B42-B46</f>
-        <v>-533</v>
+        <v>-799</v>
       </c>
       <c r="C47">
         <f>C42-C46</f>
-        <v>-178</v>
+        <v>-267</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4613,11 +4632,11 @@
       </c>
       <c r="B50">
         <f>INT(B49+(B46*$B$16)/POWER(2,9) - B47*$B$17/POWER(2,9))</f>
-        <v>1187</v>
+        <v>719</v>
       </c>
       <c r="C50">
         <f>INT(C49+(C46*$B$16)/POWER(2,9) - C47*$B$17/POWER(2,9))</f>
-        <v>1395</v>
+        <v>1239</v>
       </c>
     </row>
   </sheetData>
@@ -4630,7 +4649,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4795,7 +4814,7 @@
       <c r="A21" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>-600</v>
       </c>
     </row>
@@ -4803,7 +4822,7 @@
       <c r="A22" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <f>B21*POWER(2,1)</f>
         <v>-1200</v>
       </c>
@@ -5074,6 +5093,474 @@
       <c r="C50">
         <f>INT(C49+(C46*$B$16)/POWER(2,9) - C47*$B$17/POWER(2,9))</f>
         <v>1396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="1">
+        <v>988</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1900</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13">
+        <f>B8</f>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
+        <f>B10</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
+        <f>D10</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <f>B14-C10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <f>B15-C10</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <f>B23-C8</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27">
+        <f>ABS(B24)*POWER(2,B26)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28">
+        <f>MIN(B27,B25)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29">
+        <f>B25-B28</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31">
+        <v>400</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="D33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34">
+        <v>500</v>
+      </c>
+      <c r="F34" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35">
+        <f>-B24*POWER(2,E33)</f>
+        <v>-1600</v>
+      </c>
+      <c r="C35">
+        <f>B35</f>
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36">
+        <f>-B21</f>
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>B36</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>B38</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <f>B36-B35</f>
+        <v>1600</v>
+      </c>
+      <c r="C38">
+        <f>C36-C35</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>1600</v>
+      </c>
+      <c r="C39">
+        <f>C38-C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40">
+        <f>INT( (B38*$E$34/8+B39*$G$34/4)/POWER(2,8))</f>
+        <v>1171</v>
+      </c>
+      <c r="C40">
+        <f>INT( (C38*$E$34/8+C39*$G$34/4)/POWER(2,8))</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41">
+        <f>INT(B40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>354</v>
+      </c>
+      <c r="C41">
+        <f>INT(C40*$B$32/POWER(2,7)*$B$29/POWER(2,9)*$B$31/POWER(2,9))</f>
+        <v>118</v>
+      </c>
+      <c r="E41" t="str">
+        <f>IF((B41*B16) &gt; 0, "OK", "wrong")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43">
+        <f>$B$23</f>
+        <v>1600</v>
+      </c>
+      <c r="C43">
+        <f>$B$23</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44">
+        <f>B43+B41</f>
+        <v>1954</v>
+      </c>
+      <c r="C44">
+        <f>C43+C41</f>
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45">
+        <f>IF(B43&gt;=1500,IF(B44&gt;=1500,B41,1500-B43),IF(B44&gt;=1500,B44-1500,0))</f>
+        <v>354</v>
+      </c>
+      <c r="C45">
+        <f>IF(C43&gt;=1500,IF(C44&gt;=1500,C41,1500-C43),IF(C44&gt;=1500,C44-1500,0))</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46">
+        <f>B41-B45</f>
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f>C41-C45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48">
+        <v>1500</v>
+      </c>
+      <c r="C48">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49">
+        <f>INT(B48+(B45*$B$16)/POWER(2,9) - B46*$B$17/POWER(2,9))</f>
+        <v>1776</v>
+      </c>
+      <c r="C49">
+        <f>INT(C48+(C45*$B$16)/POWER(2,9) - C46*$B$17/POWER(2,9))</f>
+        <v>1592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>